<commit_message>
🎈 perf: add results
</commit_message>
<xml_diff>
--- a/qft_data.xlsx
+++ b/qft_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bygdc\Desktop\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D8B1794-3DEC-48B0-8A5F-52EA33B2F4C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{707349D9-C41C-41B6-BBD9-8173F0C3396B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="74">
   <si>
     <t>file_name</t>
   </si>
@@ -252,6 +252,18 @@
     <t>dynamic static</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>LNN/Enola dynamic</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LNN/Enola static</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LNN/Atomique</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -324,7 +336,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -339,13 +351,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -710,332 +725,6 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$N$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Atomique</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$3:$A$48</c:f>
-              <c:strCache>
-                <c:ptCount val="46"/>
-                <c:pt idx="0">
-                  <c:v>qft 5  fidelity</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>qft 6  fidelity</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>qft 7  fidelity</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>qft 8  fidelity</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>qft 9  fidelity</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>qft 10  fidelity</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>qft 11  fidelity</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>qft 12  fidelity</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>qft 13  fidelity</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>qft 14  fidelity</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>qft 15  fidelity</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>qft 16  fidelity</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>qft 17  fidelity</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>qft 18  fidelity</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>qft 19  fidelity</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>qft 20  fidelity</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>qft 21  fidelity</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>qft 22  fidelity</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>qft 23  fidelity</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>qft 24  fidelity</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>qft 25  fidelity</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>qft 26  fidelity</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>qft 27  fidelity</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>qft 28  fidelity</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>qft 29  fidelity</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>qft 30  fidelity</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>qft 31  fidelity</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>qft 32  fidelity</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>qft 33  fidelity</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>qft 34  fidelity</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>qft 35  fidelity</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>qft 36  fidelity</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>qft 37  fidelity</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>qft 38  fidelity</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>qft 39  fidelity</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>qft 40  fidelity</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>qft 41  fidelity</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>qft 42  fidelity</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>qft 43  fidelity</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>qft 44  fidelity</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>qft 45  fidelity</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>qft 46  fidelity</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>qft 47  fidelity</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>qft 48  fidelity</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>qft 49  fidelity</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>qft 50  fidelity</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$V$3:$V$48</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
-                <c:pt idx="0">
-                  <c:v>0.534265412008044</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.34885473842061793</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.18546173445225689</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8.0882058449014485E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4.1101208287512722E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.4336995094978019E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4.1873546106857762E-3</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7.6898597156183903E-4</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2.8923871319338118E-4</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.507017916023118E-4</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.586264509795585E-5</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4.8762918797341026E-7</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>5.5199161283621291E-8</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>3.7847064283796101E-9</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>4.4591881864229171E-10</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>9.0177467138778211E-10</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1.8375304386280249E-11</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>3.165462224454784E-13</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>4.738882334346382E-15</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>5.9916891127421894E-22</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2.7293378667521329E-19</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1.5272898152304299E-20</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>7.5622799221913974E-28</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>5.363203887401728E-30</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>4.9879018188860561E-36</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>5.1026760692481638E-42</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>1.5965314629850159E-45</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>5.2115660833410638E-47</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>2.374579795219512E-35</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>2.6441647281319418E-35</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>2.245987911150489E-37</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>5.2935714451575026E-41</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>3.3066580353319982E-53</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>3.1133640113345143E-57</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>1.9879196408487809E-46</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>1.331636708248313E-69</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>3.2128435491088098E-70</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>4.0441774501684942E-81</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>2.3340967266080449E-94</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>1.875817459152053E-77</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>2.477678759532265E-81</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>4.0908675204222109E-87</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>2.2279709957858851E-90</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>5.4270513461621089E-98</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>4.3096859133110637E-104</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>1.4996324311934879E-121</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000017-2559-411B-A81A-C5005DC24AC1}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
@@ -1689,6 +1378,356 @@
         <c:smooth val="0"/>
         <c:axId val="207500720"/>
         <c:axId val="207501136"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$N$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Atomique</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$3:$A$48</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="46"/>
+                      <c:pt idx="0">
+                        <c:v>qft 5  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>qft 6  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>qft 7  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>qft 8  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>qft 9  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>qft 10  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>qft 11  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>qft 12  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>qft 13  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>qft 14  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>qft 15  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>qft 16  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>qft 17  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>qft 18  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>qft 19  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>qft 20  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>qft 21  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>qft 22  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>qft 23  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>qft 24  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>qft 25  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>qft 26  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>qft 27  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>qft 28  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>qft 29  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>qft 30  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>qft 31  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>qft 32  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>qft 33  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>qft 34  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>qft 35  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>qft 36  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>qft 37  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>qft 38  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>qft 39  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>qft 40  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>qft 41  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>qft 42  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="38">
+                        <c:v>qft 43  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>qft 44  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="40">
+                        <c:v>qft 45  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="41">
+                        <c:v>qft 46  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="42">
+                        <c:v>qft 47  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="43">
+                        <c:v>qft 48  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="44">
+                        <c:v>qft 49  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="45">
+                        <c:v>qft 50  fidelity</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$V$3:$V$48</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="46"/>
+                      <c:pt idx="0">
+                        <c:v>0.534265412008044</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.34885473842061793</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.18546173445225689</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>8.0882058449014485E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>4.1101208287512722E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>2.4336995094978019E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>4.1873546106857762E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>7.6898597156183903E-4</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>2.8923871319338118E-4</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>1.507017916023118E-4</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>1.586264509795585E-5</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>4.8762918797341026E-7</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>5.5199161283621291E-8</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>3.7847064283796101E-9</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>4.4591881864229171E-10</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>9.0177467138778211E-10</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>1.8375304386280249E-11</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>3.165462224454784E-13</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>4.738882334346382E-15</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>5.9916891127421894E-22</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>2.7293378667521329E-19</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>1.5272898152304299E-20</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>7.5622799221913974E-28</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>5.363203887401728E-30</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>4.9879018188860561E-36</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>5.1026760692481638E-42</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>1.5965314629850159E-45</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>5.2115660833410638E-47</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>2.374579795219512E-35</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>2.6441647281319418E-35</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>2.245987911150489E-37</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>5.2935714451575026E-41</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>3.3066580353319982E-53</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>3.1133640113345143E-57</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>1.9879196408487809E-46</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>1.331636708248313E-69</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>3.2128435491088098E-70</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>4.0441774501684942E-81</c:v>
+                      </c:pt>
+                      <c:pt idx="38">
+                        <c:v>2.3340967266080449E-94</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>1.875817459152053E-77</c:v>
+                      </c:pt>
+                      <c:pt idx="40">
+                        <c:v>2.477678759532265E-81</c:v>
+                      </c:pt>
+                      <c:pt idx="41">
+                        <c:v>4.0908675204222109E-87</c:v>
+                      </c:pt>
+                      <c:pt idx="42">
+                        <c:v>2.2279709957858851E-90</c:v>
+                      </c:pt>
+                      <c:pt idx="43">
+                        <c:v>5.4270513461621089E-98</c:v>
+                      </c:pt>
+                      <c:pt idx="44">
+                        <c:v>4.3096859133110637E-104</c:v>
+                      </c:pt>
+                      <c:pt idx="45">
+                        <c:v>1.4996324311934879E-121</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000017-2559-411B-A81A-C5005DC24AC1}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
       </c:lineChart>
       <c:catAx>
         <c:axId val="207500720"/>
@@ -1848,7 +1887,1263 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AW$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LNN/Enola dynamic</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$3:$A$48</c:f>
+              <c:strCache>
+                <c:ptCount val="46"/>
+                <c:pt idx="0">
+                  <c:v>qft 5  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>qft 6  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>qft 7  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>qft 8  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>qft 9  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>qft 10  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>qft 11  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>qft 12  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>qft 13  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>qft 14  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>qft 15  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>qft 16  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>qft 17  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>qft 18  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>qft 19  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>qft 20  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>qft 21  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>qft 22  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>qft 23  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>qft 24  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>qft 25  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>qft 26  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>qft 27  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>qft 28  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>qft 29  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>qft 30  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>qft 31  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>qft 32  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>qft 33  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>qft 34  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>qft 35  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>qft 36  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>qft 37  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>qft 38  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>qft 39  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>qft 40  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>qft 41  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>qft 42  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>qft 43  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>qft 44  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>qft 45  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>qft 46  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>qft 47  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>qft 48  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>qft 49  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>qft 50  fidelity</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AW$3:$AW$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="43"/>
+                <c:pt idx="0">
+                  <c:v>0.99906468886110866</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0060528388605166</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0052300833792409</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0162976882576515</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0110751411882675</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0218075392886239</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0430358637094383</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0491904812665227</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0710336393148014</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0983565001539115</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.1501373358427713</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.1451274643608638</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.180179185938053</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.2245963710321306</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.320891794897133</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.4026601523921005</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.4340822826356749</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.7299483770757156</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.6482583286440329</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.7154822161183612</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.9896871083178245</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.1623277566983186</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.7078348945620263</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.5234874566054994</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.5174884469901424</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4.1524541448227144</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4.6746052784337788</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5.4533878876124948</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>9.2936619712897102</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>10.081364031646578</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>15.824530605514202</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>25.91101736895925</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>42.023826229752835</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>90.649361762938511</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>133.59695953750509</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>224.59850075573462</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>491.22741800560243</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1612.7594609876173</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3225.3181217713204</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>6647.6836366521375</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>24772.074844579882</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>185853.91193880278</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>375351.86648784083</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E750-4401-AF9A-AA58597206FE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AX$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LNN/Enola static</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$3:$A$48</c:f>
+              <c:strCache>
+                <c:ptCount val="46"/>
+                <c:pt idx="0">
+                  <c:v>qft 5  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>qft 6  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>qft 7  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>qft 8  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>qft 9  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>qft 10  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>qft 11  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>qft 12  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>qft 13  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>qft 14  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>qft 15  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>qft 16  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>qft 17  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>qft 18  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>qft 19  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>qft 20  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>qft 21  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>qft 22  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>qft 23  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>qft 24  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>qft 25  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>qft 26  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>qft 27  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>qft 28  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>qft 29  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>qft 30  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>qft 31  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>qft 32  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>qft 33  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>qft 34  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>qft 35  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>qft 36  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>qft 37  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>qft 38  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>qft 39  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>qft 40  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>qft 41  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>qft 42  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>qft 43  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>qft 44  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>qft 45  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>qft 46  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>qft 47  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>qft 48  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>qft 49  fidelity</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>qft 50  fidelity</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AX$3:$AX$48</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="46"/>
+                <c:pt idx="0">
+                  <c:v>1.0042047293174579</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0093223016680943</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0219832530791773</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0279176727995585</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.04221963056698</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0727784478356417</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.1145248797073457</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.1388383938149951</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.2147572225412693</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.2784539213532986</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.3791845291531124</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.4320120515472758</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.5973775294740471</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.7456542917362814</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.8824573017281718</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.2861621745759773</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.6402370406385245</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.7132429343882301</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.4674637512534132</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.7161209630610275</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4.9430773194404711</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>8.3164461329353205</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>10.256887968321816</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>12.801027489386801</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24.562936212205592</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>36.320392014835832</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>46.787182345907183</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>102.64629303406497</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>193.14237982086743</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>415.54109746281563</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1289.9709994625639</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3459.0864234780524</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>10357.038021506776</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>32195.564798304134</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>85709.052272263958</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>406986.16430719214</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1388015.8232879108</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>8505873.614096839</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>80077488.064241618</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>770943307.52212453</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>25760128288.775894</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>37197454244.013763</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4934782166036.6924</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>98349781865872.469</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.0053759805058516E+16</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>7.1474179843793869E+17</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-E750-4401-AF9A-AA58597206FE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1869100096"/>
+        <c:axId val="1869100512"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$AV$2</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>LNN/Atomique</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$3:$A$48</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="46"/>
+                      <c:pt idx="0">
+                        <c:v>qft 5  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>qft 6  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>qft 7  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>qft 8  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>qft 9  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>qft 10  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>qft 11  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>qft 12  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>qft 13  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>qft 14  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>qft 15  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>qft 16  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>qft 17  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>qft 18  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>qft 19  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>qft 20  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>qft 21  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>qft 22  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>qft 23  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>qft 24  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>qft 25  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>qft 26  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>qft 27  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>qft 28  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>qft 29  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>qft 30  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>qft 31  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>qft 32  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>qft 33  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>qft 34  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>qft 35  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>qft 36  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>qft 37  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>qft 38  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>qft 39  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>qft 40  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>qft 41  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>qft 42  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="38">
+                        <c:v>qft 43  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>qft 44  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="40">
+                        <c:v>qft 45  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="41">
+                        <c:v>qft 46  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="42">
+                        <c:v>qft 47  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="43">
+                        <c:v>qft 48  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="44">
+                        <c:v>qft 49  fidelity</c:v>
+                      </c:pt>
+                      <c:pt idx="45">
+                        <c:v>qft 50  fidelity</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$AV$3:$AV$48</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="46"/>
+                      <c:pt idx="0">
+                        <c:v>1.4206170770953306</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1.8689379480747979</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>2.9171074324190136</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>5.356785377477979</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>8.1393816371485777</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>10.217043025632602</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>42.498453688605942</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>159.1881978696876</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>279.42072175506217</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>339.54613582188523</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>1956.4429392673776</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>36931.536183970187</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>181097.31683488714</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>1395326.9824050723</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>5978547.8624049192</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>1420965.8362082948</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>31850900.953618295</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>801810231.81761694</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>22021015217.798889</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>6.776052501398688E+16</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>54591995302255.32</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>339162871928041.25</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>2.2479993037699854E+21</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>9.9007983128765522E+22</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>3.1877131060993765E+28</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>8.8776946420340919E+33</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>7.7042014424212072E+36</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>6.1593769486313655E+37</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>3.3605945843830065E+25</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>7.0721766314503553E+24</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>1.8833583115027618E+26</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>1.7133989961157756E+29</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>5.5947726684542223E+40</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>1.1530935627604882E+44</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>3.3250841050988021E+32</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>8.7110845834665328E+54</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>5.9760146133868756E+54</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>7.4675259362671538E+64</c:v>
+                      </c:pt>
+                      <c:pt idx="38">
+                        <c:v>1.9322249796194267E+77</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>3.40651483374536E+59</c:v>
+                      </c:pt>
+                      <c:pt idx="40">
+                        <c:v>3.4467745130979681E+62</c:v>
+                      </c:pt>
+                      <c:pt idx="41">
+                        <c:v>2.6400268270934748E+67</c:v>
+                      </c:pt>
+                      <c:pt idx="42">
+                        <c:v>5.7900215148221476E+69</c:v>
+                      </c:pt>
+                      <c:pt idx="43">
+                        <c:v>2.6718007763560374E+76</c:v>
+                      </c:pt>
+                      <c:pt idx="44">
+                        <c:v>3.5965497977767005E+81</c:v>
+                      </c:pt>
+                      <c:pt idx="45">
+                        <c:v>1.0202500080518689E+98</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-E750-4401-AF9A-AA58597206FE}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1869100096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="t"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1869100512"/>
+        <c:crosses val="max"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1869100512"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1869100096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2404,19 +3699,535 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>548640</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>396240</xdr:colOff>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>243840</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>396240</xdr:colOff>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>34290</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2437,6 +4248,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1142999</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>157843</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>152399</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="图表 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B70C0BE2-DDB2-434C-A50F-51BC69BF42B2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2708,73 +4555,78 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AT48"/>
+  <dimension ref="A1:AX48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AV2" sqref="AV2:AX48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18.88671875" bestFit="1" customWidth="1"/>
     <col min="24" max="34" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A1" s="8"/>
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A1" s="6"/>
+      <c r="B1" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="N1" s="6" t="s">
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="N1" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="X1" s="7" t="s">
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="X1" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="Y1" s="7"/>
-      <c r="Z1" s="7"/>
-      <c r="AA1" s="7"/>
-      <c r="AB1" s="7"/>
-      <c r="AC1" s="7"/>
-      <c r="AD1" s="7"/>
-      <c r="AE1" s="7"/>
-      <c r="AF1" s="7"/>
-      <c r="AG1" s="7"/>
-      <c r="AH1" s="7"/>
-      <c r="AJ1" s="5" t="s">
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="8"/>
+      <c r="AA1" s="8"/>
+      <c r="AB1" s="8"/>
+      <c r="AC1" s="8"/>
+      <c r="AD1" s="8"/>
+      <c r="AE1" s="8"/>
+      <c r="AF1" s="8"/>
+      <c r="AG1" s="8"/>
+      <c r="AH1" s="8"/>
+      <c r="AJ1" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="AK1" s="5"/>
-      <c r="AL1" s="5"/>
-      <c r="AM1" s="5"/>
-      <c r="AN1" s="5"/>
-      <c r="AO1" s="5"/>
-      <c r="AP1" s="5"/>
-      <c r="AQ1" s="5"/>
-      <c r="AR1" s="5"/>
-      <c r="AS1" s="5"/>
-      <c r="AT1" s="5"/>
+      <c r="AK1" s="9"/>
+      <c r="AL1" s="9"/>
+      <c r="AM1" s="9"/>
+      <c r="AN1" s="9"/>
+      <c r="AO1" s="9"/>
+      <c r="AP1" s="9"/>
+      <c r="AQ1" s="9"/>
+      <c r="AR1" s="9"/>
+      <c r="AS1" s="9"/>
+      <c r="AT1" s="9"/>
+      <c r="AU1" s="5"/>
     </row>
-    <row r="2" spans="1:46" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:50" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2904,8 +4756,18 @@
       <c r="AT2" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="AU2" s="3"/>
+      <c r="AV2" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AW2" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AX2" s="3" t="s">
+        <v>72</v>
+      </c>
     </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -3035,8 +4897,21 @@
       <c r="AT3" s="3">
         <v>43.118530179255501</v>
       </c>
+      <c r="AU3" s="3"/>
+      <c r="AV3">
+        <f>B3/V3</f>
+        <v>1.4206170770953306</v>
+      </c>
+      <c r="AW3">
+        <f>B3/X3</f>
+        <v>0.99906468886110866</v>
+      </c>
+      <c r="AX3">
+        <f>B3/AJ3</f>
+        <v>1.0042047293174579</v>
+      </c>
     </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -3166,8 +5041,21 @@
       <c r="AT4" s="3">
         <v>43.799459931563497</v>
       </c>
+      <c r="AU4" s="3"/>
+      <c r="AV4">
+        <f t="shared" ref="AV4:AV48" si="0">B4/V4</f>
+        <v>1.8689379480747979</v>
+      </c>
+      <c r="AW4">
+        <f t="shared" ref="AW4:AW45" si="1">B4/X4</f>
+        <v>1.0060528388605166</v>
+      </c>
+      <c r="AX4">
+        <f t="shared" ref="AX4:AX48" si="2">B4/AJ4</f>
+        <v>1.0093223016680943</v>
+      </c>
     </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -3297,8 +5185,21 @@
       <c r="AT5" s="3">
         <v>44.066267866319698</v>
       </c>
+      <c r="AU5" s="3"/>
+      <c r="AV5">
+        <f t="shared" si="0"/>
+        <v>2.9171074324190136</v>
+      </c>
+      <c r="AW5">
+        <f t="shared" si="1"/>
+        <v>1.0052300833792409</v>
+      </c>
+      <c r="AX5">
+        <f t="shared" si="2"/>
+        <v>1.0219832530791773</v>
+      </c>
     </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -3428,8 +5329,21 @@
       <c r="AT6" s="3">
         <v>45.691856692490603</v>
       </c>
+      <c r="AU6" s="3"/>
+      <c r="AV6">
+        <f t="shared" si="0"/>
+        <v>5.356785377477979</v>
+      </c>
+      <c r="AW6">
+        <f t="shared" si="1"/>
+        <v>1.0162976882576515</v>
+      </c>
+      <c r="AX6">
+        <f t="shared" si="2"/>
+        <v>1.0279176727995585</v>
+      </c>
     </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -3559,8 +5473,21 @@
       <c r="AT7" s="3">
         <v>45.235360638034898</v>
       </c>
+      <c r="AU7" s="3"/>
+      <c r="AV7">
+        <f t="shared" si="0"/>
+        <v>8.1393816371485777</v>
+      </c>
+      <c r="AW7">
+        <f t="shared" si="1"/>
+        <v>1.0110751411882675</v>
+      </c>
+      <c r="AX7">
+        <f t="shared" si="2"/>
+        <v>1.04221963056698</v>
+      </c>
     </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -3690,8 +5617,21 @@
       <c r="AT8" s="3">
         <v>45.506002416504003</v>
       </c>
+      <c r="AU8" s="3"/>
+      <c r="AV8">
+        <f t="shared" si="0"/>
+        <v>10.217043025632602</v>
+      </c>
+      <c r="AW8">
+        <f t="shared" si="1"/>
+        <v>1.0218075392886239</v>
+      </c>
+      <c r="AX8">
+        <f t="shared" si="2"/>
+        <v>1.0727784478356417</v>
+      </c>
     </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -3821,8 +5761,21 @@
       <c r="AT9" s="3">
         <v>47.014815196838299</v>
       </c>
+      <c r="AU9" s="3"/>
+      <c r="AV9">
+        <f t="shared" si="0"/>
+        <v>42.498453688605942</v>
+      </c>
+      <c r="AW9">
+        <f t="shared" si="1"/>
+        <v>1.0430358637094383</v>
+      </c>
+      <c r="AX9">
+        <f t="shared" si="2"/>
+        <v>1.1145248797073457</v>
+      </c>
     </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -3952,8 +5905,21 @@
       <c r="AT10" s="3">
         <v>46.743978382869798</v>
       </c>
+      <c r="AU10" s="3"/>
+      <c r="AV10">
+        <f t="shared" si="0"/>
+        <v>159.1881978696876</v>
+      </c>
+      <c r="AW10">
+        <f t="shared" si="1"/>
+        <v>1.0491904812665227</v>
+      </c>
+      <c r="AX10">
+        <f t="shared" si="2"/>
+        <v>1.1388383938149951</v>
+      </c>
     </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -4083,8 +6049,21 @@
       <c r="AT11" s="3">
         <v>46.516996652102797</v>
       </c>
+      <c r="AU11" s="3"/>
+      <c r="AV11">
+        <f t="shared" si="0"/>
+        <v>279.42072175506217</v>
+      </c>
+      <c r="AW11">
+        <f t="shared" si="1"/>
+        <v>1.0710336393148014</v>
+      </c>
+      <c r="AX11">
+        <f t="shared" si="2"/>
+        <v>1.2147572225412693</v>
+      </c>
     </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -4214,8 +6193,21 @@
       <c r="AT12" s="3">
         <v>46.250812192205601</v>
       </c>
+      <c r="AU12" s="3"/>
+      <c r="AV12">
+        <f t="shared" si="0"/>
+        <v>339.54613582188523</v>
+      </c>
+      <c r="AW12">
+        <f t="shared" si="1"/>
+        <v>1.0983565001539115</v>
+      </c>
+      <c r="AX12">
+        <f t="shared" si="2"/>
+        <v>1.2784539213532986</v>
+      </c>
     </row>
-    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -4345,8 +6337,21 @@
       <c r="AT13" s="3">
         <v>46.837669042303602</v>
       </c>
+      <c r="AU13" s="3"/>
+      <c r="AV13">
+        <f t="shared" si="0"/>
+        <v>1956.4429392673776</v>
+      </c>
+      <c r="AW13">
+        <f t="shared" si="1"/>
+        <v>1.1501373358427713</v>
+      </c>
+      <c r="AX13">
+        <f t="shared" si="2"/>
+        <v>1.3791845291531124</v>
+      </c>
     </row>
-    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -4476,8 +6481,21 @@
       <c r="AT14" s="3">
         <v>47.097167383152403</v>
       </c>
+      <c r="AU14" s="3"/>
+      <c r="AV14">
+        <f t="shared" si="0"/>
+        <v>36931.536183970187</v>
+      </c>
+      <c r="AW14">
+        <f t="shared" si="1"/>
+        <v>1.1451274643608638</v>
+      </c>
+      <c r="AX14">
+        <f t="shared" si="2"/>
+        <v>1.4320120515472758</v>
+      </c>
     </row>
-    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -4607,8 +6625,21 @@
       <c r="AT15" s="3">
         <v>48.283906751172097</v>
       </c>
+      <c r="AU15" s="3"/>
+      <c r="AV15">
+        <f t="shared" si="0"/>
+        <v>181097.31683488714</v>
+      </c>
+      <c r="AW15">
+        <f t="shared" si="1"/>
+        <v>1.180179185938053</v>
+      </c>
+      <c r="AX15">
+        <f t="shared" si="2"/>
+        <v>1.5973775294740471</v>
+      </c>
     </row>
-    <row r="16" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -4738,8 +6769,21 @@
       <c r="AT16" s="3">
         <v>47.5682386920409</v>
       </c>
+      <c r="AU16" s="3"/>
+      <c r="AV16">
+        <f t="shared" si="0"/>
+        <v>1395326.9824050723</v>
+      </c>
+      <c r="AW16">
+        <f t="shared" si="1"/>
+        <v>1.2245963710321306</v>
+      </c>
+      <c r="AX16">
+        <f t="shared" si="2"/>
+        <v>1.7456542917362814</v>
+      </c>
     </row>
-    <row r="17" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -4869,8 +6913,21 @@
       <c r="AT17" s="3">
         <v>48.018219860255002</v>
       </c>
+      <c r="AU17" s="3"/>
+      <c r="AV17">
+        <f t="shared" si="0"/>
+        <v>5978547.8624049192</v>
+      </c>
+      <c r="AW17">
+        <f t="shared" si="1"/>
+        <v>1.320891794897133</v>
+      </c>
+      <c r="AX17">
+        <f t="shared" si="2"/>
+        <v>1.8824573017281718</v>
+      </c>
     </row>
-    <row r="18" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -5000,8 +7057,21 @@
       <c r="AT18" s="3">
         <v>48.123342424218599</v>
       </c>
+      <c r="AU18" s="3"/>
+      <c r="AV18">
+        <f t="shared" si="0"/>
+        <v>1420965.8362082948</v>
+      </c>
+      <c r="AW18">
+        <f t="shared" si="1"/>
+        <v>1.4026601523921005</v>
+      </c>
+      <c r="AX18">
+        <f t="shared" si="2"/>
+        <v>2.2861621745759773</v>
+      </c>
     </row>
-    <row r="19" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>28</v>
       </c>
@@ -5131,8 +7201,21 @@
       <c r="AT19" s="3">
         <v>47.745644454218102</v>
       </c>
+      <c r="AU19" s="3"/>
+      <c r="AV19">
+        <f t="shared" si="0"/>
+        <v>31850900.953618295</v>
+      </c>
+      <c r="AW19">
+        <f t="shared" si="1"/>
+        <v>1.4340822826356749</v>
+      </c>
+      <c r="AX19">
+        <f t="shared" si="2"/>
+        <v>2.6402370406385245</v>
+      </c>
     </row>
-    <row r="20" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -5262,8 +7345,21 @@
       <c r="AT20" s="3">
         <v>47.947967097442103</v>
       </c>
+      <c r="AU20" s="3"/>
+      <c r="AV20">
+        <f t="shared" si="0"/>
+        <v>801810231.81761694</v>
+      </c>
+      <c r="AW20">
+        <f t="shared" si="1"/>
+        <v>1.7299483770757156</v>
+      </c>
+      <c r="AX20">
+        <f t="shared" si="2"/>
+        <v>2.7132429343882301</v>
+      </c>
     </row>
-    <row r="21" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -5393,8 +7489,21 @@
       <c r="AT21" s="3">
         <v>47.657689369446302</v>
       </c>
+      <c r="AU21" s="3"/>
+      <c r="AV21">
+        <f t="shared" si="0"/>
+        <v>22021015217.798889</v>
+      </c>
+      <c r="AW21">
+        <f t="shared" si="1"/>
+        <v>1.6482583286440329</v>
+      </c>
+      <c r="AX21">
+        <f t="shared" si="2"/>
+        <v>3.4674637512534132</v>
+      </c>
     </row>
-    <row r="22" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -5524,8 +7633,21 @@
       <c r="AT22" s="3">
         <v>49.068561183243702</v>
       </c>
+      <c r="AU22" s="3"/>
+      <c r="AV22">
+        <f t="shared" si="0"/>
+        <v>6.776052501398688E+16</v>
+      </c>
+      <c r="AW22">
+        <f t="shared" si="1"/>
+        <v>1.7154822161183612</v>
+      </c>
+      <c r="AX22">
+        <f t="shared" si="2"/>
+        <v>4.7161209630610275</v>
+      </c>
     </row>
-    <row r="23" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>32</v>
       </c>
@@ -5655,8 +7777,21 @@
       <c r="AT23" s="3">
         <v>47.720491030873099</v>
       </c>
+      <c r="AU23" s="3"/>
+      <c r="AV23">
+        <f t="shared" si="0"/>
+        <v>54591995302255.32</v>
+      </c>
+      <c r="AW23">
+        <f t="shared" si="1"/>
+        <v>1.9896871083178245</v>
+      </c>
+      <c r="AX23">
+        <f t="shared" si="2"/>
+        <v>4.9430773194404711</v>
+      </c>
     </row>
-    <row r="24" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -5786,8 +7921,21 @@
       <c r="AT24" s="3">
         <v>48.630284106141801</v>
       </c>
+      <c r="AU24" s="3"/>
+      <c r="AV24">
+        <f t="shared" si="0"/>
+        <v>339162871928041.25</v>
+      </c>
+      <c r="AW24">
+        <f t="shared" si="1"/>
+        <v>2.1623277566983186</v>
+      </c>
+      <c r="AX24">
+        <f t="shared" si="2"/>
+        <v>8.3164461329353205</v>
+      </c>
     </row>
-    <row r="25" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -5917,8 +8065,21 @@
       <c r="AT25" s="3">
         <v>48.920362246726597</v>
       </c>
+      <c r="AU25" s="3"/>
+      <c r="AV25">
+        <f t="shared" si="0"/>
+        <v>2.2479993037699854E+21</v>
+      </c>
+      <c r="AW25">
+        <f t="shared" si="1"/>
+        <v>2.7078348945620263</v>
+      </c>
+      <c r="AX25">
+        <f t="shared" si="2"/>
+        <v>10.256887968321816</v>
+      </c>
     </row>
-    <row r="26" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>35</v>
       </c>
@@ -6048,8 +8209,21 @@
       <c r="AT26" s="3">
         <v>48.754502961000298</v>
       </c>
+      <c r="AU26" s="3"/>
+      <c r="AV26">
+        <f t="shared" si="0"/>
+        <v>9.9007983128765522E+22</v>
+      </c>
+      <c r="AW26">
+        <f t="shared" si="1"/>
+        <v>2.5234874566054994</v>
+      </c>
+      <c r="AX26">
+        <f t="shared" si="2"/>
+        <v>12.801027489386801</v>
+      </c>
     </row>
-    <row r="27" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>36</v>
       </c>
@@ -6179,8 +8353,21 @@
       <c r="AT27" s="3">
         <v>49.053258295232602</v>
       </c>
+      <c r="AU27" s="3"/>
+      <c r="AV27">
+        <f t="shared" si="0"/>
+        <v>3.1877131060993765E+28</v>
+      </c>
+      <c r="AW27">
+        <f t="shared" si="1"/>
+        <v>2.5174884469901424</v>
+      </c>
+      <c r="AX27">
+        <f t="shared" si="2"/>
+        <v>24.562936212205592</v>
+      </c>
     </row>
-    <row r="28" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>37</v>
       </c>
@@ -6310,8 +8497,21 @@
       <c r="AT28" s="3">
         <v>49.239122258391198</v>
       </c>
+      <c r="AU28" s="3"/>
+      <c r="AV28">
+        <f t="shared" si="0"/>
+        <v>8.8776946420340919E+33</v>
+      </c>
+      <c r="AW28">
+        <f t="shared" si="1"/>
+        <v>4.1524541448227144</v>
+      </c>
+      <c r="AX28">
+        <f t="shared" si="2"/>
+        <v>36.320392014835832</v>
+      </c>
     </row>
-    <row r="29" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>38</v>
       </c>
@@ -6441,8 +8641,21 @@
       <c r="AT29" s="3">
         <v>49.252981396323698</v>
       </c>
+      <c r="AU29" s="3"/>
+      <c r="AV29">
+        <f t="shared" si="0"/>
+        <v>7.7042014424212072E+36</v>
+      </c>
+      <c r="AW29">
+        <f t="shared" si="1"/>
+        <v>4.6746052784337788</v>
+      </c>
+      <c r="AX29">
+        <f t="shared" si="2"/>
+        <v>46.787182345907183</v>
+      </c>
     </row>
-    <row r="30" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>39</v>
       </c>
@@ -6572,8 +8785,21 @@
       <c r="AT30" s="3">
         <v>49.197348245816997</v>
       </c>
+      <c r="AU30" s="3"/>
+      <c r="AV30">
+        <f t="shared" si="0"/>
+        <v>6.1593769486313655E+37</v>
+      </c>
+      <c r="AW30">
+        <f t="shared" si="1"/>
+        <v>5.4533878876124948</v>
+      </c>
+      <c r="AX30">
+        <f t="shared" si="2"/>
+        <v>102.64629303406497</v>
+      </c>
     </row>
-    <row r="31" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>40</v>
       </c>
@@ -6703,8 +8929,21 @@
       <c r="AT31" s="3">
         <v>49.228097730483903</v>
       </c>
+      <c r="AU31" s="3"/>
+      <c r="AV31">
+        <f t="shared" si="0"/>
+        <v>3.3605945843830065E+25</v>
+      </c>
+      <c r="AW31">
+        <f t="shared" si="1"/>
+        <v>9.2936619712897102</v>
+      </c>
+      <c r="AX31">
+        <f t="shared" si="2"/>
+        <v>193.14237982086743</v>
+      </c>
     </row>
-    <row r="32" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>41</v>
       </c>
@@ -6834,8 +9073,21 @@
       <c r="AT32" s="3">
         <v>50.391299080517101</v>
       </c>
+      <c r="AU32" s="3"/>
+      <c r="AV32">
+        <f t="shared" si="0"/>
+        <v>7.0721766314503553E+24</v>
+      </c>
+      <c r="AW32">
+        <f t="shared" si="1"/>
+        <v>10.081364031646578</v>
+      </c>
+      <c r="AX32">
+        <f t="shared" si="2"/>
+        <v>415.54109746281563</v>
+      </c>
     </row>
-    <row r="33" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>42</v>
       </c>
@@ -6965,8 +9217,21 @@
       <c r="AT33" s="3">
         <v>49.998515642688403</v>
       </c>
+      <c r="AU33" s="3"/>
+      <c r="AV33">
+        <f t="shared" si="0"/>
+        <v>1.8833583115027618E+26</v>
+      </c>
+      <c r="AW33">
+        <f t="shared" si="1"/>
+        <v>15.824530605514202</v>
+      </c>
+      <c r="AX33">
+        <f t="shared" si="2"/>
+        <v>1289.9709994625639</v>
+      </c>
     </row>
-    <row r="34" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>43</v>
       </c>
@@ -7096,8 +9361,21 @@
       <c r="AT34" s="3">
         <v>50.225235408135902</v>
       </c>
+      <c r="AU34" s="3"/>
+      <c r="AV34">
+        <f t="shared" si="0"/>
+        <v>1.7133989961157756E+29</v>
+      </c>
+      <c r="AW34">
+        <f t="shared" si="1"/>
+        <v>25.91101736895925</v>
+      </c>
+      <c r="AX34">
+        <f t="shared" si="2"/>
+        <v>3459.0864234780524</v>
+      </c>
     </row>
-    <row r="35" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>44</v>
       </c>
@@ -7227,8 +9505,21 @@
       <c r="AT35" s="3">
         <v>50.222968045733403</v>
       </c>
+      <c r="AU35" s="3"/>
+      <c r="AV35">
+        <f t="shared" si="0"/>
+        <v>5.5947726684542223E+40</v>
+      </c>
+      <c r="AW35">
+        <f t="shared" si="1"/>
+        <v>42.023826229752835</v>
+      </c>
+      <c r="AX35">
+        <f t="shared" si="2"/>
+        <v>10357.038021506776</v>
+      </c>
     </row>
-    <row r="36" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>45</v>
       </c>
@@ -7358,8 +9649,21 @@
       <c r="AT36" s="3">
         <v>50.200125964237301</v>
       </c>
+      <c r="AU36" s="3"/>
+      <c r="AV36">
+        <f t="shared" si="0"/>
+        <v>1.1530935627604882E+44</v>
+      </c>
+      <c r="AW36">
+        <f t="shared" si="1"/>
+        <v>90.649361762938511</v>
+      </c>
+      <c r="AX36">
+        <f t="shared" si="2"/>
+        <v>32195.564798304134</v>
+      </c>
     </row>
-    <row r="37" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>46</v>
       </c>
@@ -7489,8 +9793,21 @@
       <c r="AT37" s="3">
         <v>49.955772596840298</v>
       </c>
+      <c r="AU37" s="3"/>
+      <c r="AV37">
+        <f t="shared" si="0"/>
+        <v>3.3250841050988021E+32</v>
+      </c>
+      <c r="AW37">
+        <f t="shared" si="1"/>
+        <v>133.59695953750509</v>
+      </c>
+      <c r="AX37">
+        <f t="shared" si="2"/>
+        <v>85709.052272263958</v>
+      </c>
     </row>
-    <row r="38" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>47</v>
       </c>
@@ -7620,8 +9937,21 @@
       <c r="AT38" s="3">
         <v>50.198427154349297</v>
       </c>
+      <c r="AU38" s="3"/>
+      <c r="AV38">
+        <f t="shared" si="0"/>
+        <v>8.7110845834665328E+54</v>
+      </c>
+      <c r="AW38">
+        <f t="shared" si="1"/>
+        <v>224.59850075573462</v>
+      </c>
+      <c r="AX38">
+        <f t="shared" si="2"/>
+        <v>406986.16430719214</v>
+      </c>
     </row>
-    <row r="39" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>48</v>
       </c>
@@ -7751,8 +10081,21 @@
       <c r="AT39" s="3">
         <v>50.046830199814202</v>
       </c>
+      <c r="AU39" s="3"/>
+      <c r="AV39">
+        <f t="shared" si="0"/>
+        <v>5.9760146133868756E+54</v>
+      </c>
+      <c r="AW39">
+        <f t="shared" si="1"/>
+        <v>491.22741800560243</v>
+      </c>
+      <c r="AX39">
+        <f t="shared" si="2"/>
+        <v>1388015.8232879108</v>
+      </c>
     </row>
-    <row r="40" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>49</v>
       </c>
@@ -7882,8 +10225,21 @@
       <c r="AT40" s="3">
         <v>50.295597713488199</v>
       </c>
+      <c r="AU40" s="3"/>
+      <c r="AV40">
+        <f t="shared" si="0"/>
+        <v>7.4675259362671538E+64</v>
+      </c>
+      <c r="AW40">
+        <f t="shared" si="1"/>
+        <v>1612.7594609876173</v>
+      </c>
+      <c r="AX40">
+        <f t="shared" si="2"/>
+        <v>8505873.614096839</v>
+      </c>
     </row>
-    <row r="41" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>50</v>
       </c>
@@ -8013,8 +10369,21 @@
       <c r="AT41" s="3">
         <v>50.745339607579197</v>
       </c>
+      <c r="AU41" s="3"/>
+      <c r="AV41">
+        <f t="shared" si="0"/>
+        <v>1.9322249796194267E+77</v>
+      </c>
+      <c r="AW41">
+        <f t="shared" si="1"/>
+        <v>3225.3181217713204</v>
+      </c>
+      <c r="AX41">
+        <f t="shared" si="2"/>
+        <v>80077488.064241618</v>
+      </c>
     </row>
-    <row r="42" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>51</v>
       </c>
@@ -8144,8 +10513,21 @@
       <c r="AT42" s="3">
         <v>50.802780551236097</v>
       </c>
+      <c r="AU42" s="3"/>
+      <c r="AV42">
+        <f t="shared" si="0"/>
+        <v>3.40651483374536E+59</v>
+      </c>
+      <c r="AW42">
+        <f t="shared" si="1"/>
+        <v>6647.6836366521375</v>
+      </c>
+      <c r="AX42">
+        <f t="shared" si="2"/>
+        <v>770943307.52212453</v>
+      </c>
     </row>
-    <row r="43" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>52</v>
       </c>
@@ -8275,8 +10657,21 @@
       <c r="AT43" s="3">
         <v>50.967015243198801</v>
       </c>
+      <c r="AU43" s="3"/>
+      <c r="AV43">
+        <f t="shared" si="0"/>
+        <v>3.4467745130979681E+62</v>
+      </c>
+      <c r="AW43">
+        <f t="shared" si="1"/>
+        <v>24772.074844579882</v>
+      </c>
+      <c r="AX43">
+        <f t="shared" si="2"/>
+        <v>25760128288.775894</v>
+      </c>
     </row>
-    <row r="44" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>53</v>
       </c>
@@ -8406,8 +10801,21 @@
       <c r="AT44" s="3">
         <v>50.536820529896097</v>
       </c>
+      <c r="AU44" s="3"/>
+      <c r="AV44">
+        <f t="shared" si="0"/>
+        <v>2.6400268270934748E+67</v>
+      </c>
+      <c r="AW44">
+        <f t="shared" si="1"/>
+        <v>185853.91193880278</v>
+      </c>
+      <c r="AX44">
+        <f t="shared" si="2"/>
+        <v>37197454244.013763</v>
+      </c>
     </row>
-    <row r="45" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>54</v>
       </c>
@@ -8537,8 +10945,21 @@
       <c r="AT45" s="3">
         <v>50.477803100772597</v>
       </c>
+      <c r="AU45" s="3"/>
+      <c r="AV45">
+        <f t="shared" si="0"/>
+        <v>5.7900215148221476E+69</v>
+      </c>
+      <c r="AW45">
+        <f t="shared" si="1"/>
+        <v>375351.86648784083</v>
+      </c>
+      <c r="AX45">
+        <f t="shared" si="2"/>
+        <v>4934782166036.6924</v>
+      </c>
     </row>
-    <row r="46" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>55</v>
       </c>
@@ -8635,8 +11056,17 @@
       <c r="AT46" s="3">
         <v>50.804403734456002</v>
       </c>
+      <c r="AU46" s="3"/>
+      <c r="AV46">
+        <f t="shared" si="0"/>
+        <v>2.6718007763560374E+76</v>
+      </c>
+      <c r="AX46">
+        <f t="shared" si="2"/>
+        <v>98349781865872.469</v>
+      </c>
     </row>
-    <row r="47" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>56</v>
       </c>
@@ -8733,8 +11163,17 @@
       <c r="AT47" s="3">
         <v>50.908642114236997</v>
       </c>
+      <c r="AU47" s="3"/>
+      <c r="AV47">
+        <f t="shared" si="0"/>
+        <v>3.5965497977767005E+81</v>
+      </c>
+      <c r="AX47">
+        <f t="shared" si="2"/>
+        <v>1.0053759805058516E+16</v>
+      </c>
     </row>
-    <row r="48" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>57</v>
       </c>
@@ -8830,6 +11269,15 @@
       </c>
       <c r="AT48" s="3">
         <v>50.781013340393798</v>
+      </c>
+      <c r="AU48" s="3"/>
+      <c r="AV48">
+        <f t="shared" si="0"/>
+        <v>1.0202500080518689E+98</v>
+      </c>
+      <c r="AX48">
+        <f t="shared" si="2"/>
+        <v>7.1474179843793869E+17</v>
       </c>
     </row>
   </sheetData>
@@ -8841,6 +11289,7 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>